<commit_message>
Collision fixed og Bot movement bedre
</commit_message>
<xml_diff>
--- a/Skriftlige Produkter/Tidsplan.xlsx
+++ b/Skriftlige Produkter/Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Life-Of-Mark---After-Iteration-0\Skriftlige Produkter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78987EC-4AF0-45D8-BE92-23782EEBFBC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A72B74-F29C-4E8E-A41D-BBE70AEFD245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CFF20DE-F54B-4CA7-9EA6-B3F70A24F71B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Dato</t>
   </si>
@@ -107,15 +107,9 @@
     <t xml:space="preserve">Collision + hitbox </t>
   </si>
   <si>
-    <t xml:space="preserve">Sceneskift, Kampanimationer (evt helt kampsystem), Ryddet op i classes,            Hitboxes og collision, </t>
-  </si>
-  <si>
     <t>DEADLINE FOR ITERATION 1!!!</t>
   </si>
   <si>
-    <t>Save-system, Arbejde på historie</t>
-  </si>
-  <si>
     <t>Forbered og fuldfør iteration 1 aflevering              +                      Nyt Game koncept</t>
   </si>
   <si>
@@ -126,13 +120,87 @@
   </si>
   <si>
     <t>Kampsystem og AI</t>
+  </si>
+  <si>
+    <t>Kampanimationer og AI-movement</t>
+  </si>
+  <si>
+    <t>Kampsystem (AI)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Save-system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Arbejde på historie</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sceneskift, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kampanimationer (evt helt kampsystem)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Ryddet op i classes,            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hitboxes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> og collision, </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +224,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -279,6 +369,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89B9FC7-9091-471F-B5D0-05011EE7CF83}">
   <dimension ref="A1:X98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +938,7 @@
         <v>43905</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>21</v>
@@ -859,7 +952,7 @@
         <v>43906</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -867,7 +960,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="J21" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,7 +968,7 @@
         <v>43907</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,8 +985,8 @@
       <c r="A25" s="1">
         <v>43910</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
+      <c r="B25" s="24" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -940,8 +1033,8 @@
       <c r="A34" s="5">
         <v>43919</v>
       </c>
-      <c r="B34" t="s">
-        <v>30</v>
+      <c r="B34" s="24" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -963,6 +1056,9 @@
       <c r="A38" s="13">
         <v>43923</v>
       </c>
+      <c r="B38" s="25" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="39" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
@@ -988,6 +1084,9 @@
       <c r="A43" s="13">
         <v>43928</v>
       </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="44" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
@@ -1049,7 +1148,7 @@
         <v>43940</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>